<commit_message>
Poprawka, literówki wyszły przy imporcie
</commit_message>
<xml_diff>
--- a/doc/schemas_v2_VW/Sprzedawcy detaliczni v2.xlsx
+++ b/doc/schemas_v2_VW/Sprzedawcy detaliczni v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="APSY" sheetId="1" state="visible" r:id="rId2"/>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Trudne sytuacje, a dobre doświadczenia</t>
   </si>
   <si>
-    <t xml:space="preserve">b6,b7.b8.b9</t>
+    <t xml:space="preserve">b6,b7,b8,b9</t>
   </si>
   <si>
     <t xml:space="preserve">re</t>
@@ -400,7 +400,7 @@
     • Kompetencje: Komunikacja + Budowanie relacji.</t>
   </si>
   <si>
-    <t xml:space="preserve">201001,201002201003,201004,201005,201006,201007,201008,201009</t>
+    <t xml:space="preserve">201001,201002,201003,201004,201005,201006,201007,201008,201009</t>
   </si>
   <si>
     <t xml:space="preserve">b2</t>
@@ -1617,7 +1617,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1781,8 +1781,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1954,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2265,7 +2265,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="181.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>89</v>
       </c>
@@ -2834,8 +2834,8 @@
   </sheetPr>
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>